<commit_message>
Project - 2 iteration
</commit_message>
<xml_diff>
--- a/Project/technology.xlsx
+++ b/Project/technology.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,52 +424,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Обозначение</t>
+          <t>ОБОЗНАЧЕНИЕ</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Наименование</t>
+          <t>НАИМЕНОВАНИЕ</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Маршрут</t>
+          <t>МАРШРУТ</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Входимость</t>
+          <t>ВХОДИМОСТЬ</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Партия</t>
+          <t>ПАРТИЯ</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Цена за шт.</t>
+          <t>ЦЕНА за шт.</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Цена за комплект</t>
+          <t>ЦЕНА за комплект</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>№ операции</t>
+          <t>№ ОПЕРАЦИИ</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Наименование операции</t>
+          <t>НАИМЕНОВАНИЕ ОПЕРАЦИИ</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Оборудование</t>
+          <t>ОБОРУДОВАНИЕ</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
@@ -509,6 +509,174 @@
       </c>
       <c r="E2" t="n">
         <v>50</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>5,5</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>QWP</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>QWP</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>6,0</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0,25</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>OP80</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>OP90</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>OP80</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>OP90</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project - 2 iteration - correction
</commit_message>
<xml_diff>
--- a/Project/technology.xlsx
+++ b/Project/technology.xlsx
@@ -474,12 +474,12 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Тпз</t>
+          <t>Тпз, мин</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Тшт</t>
+          <t>Тшт, мин</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">

</xml_diff>

<commit_message>
Project - final iteration
</commit_message>
<xml_diff>
--- a/Project/technology.xlsx
+++ b/Project/technology.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,17 +491,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DA08-00.0100.01</t>
+          <t>DA08-00.0100.02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Фланец передний</t>
+          <t>Корпус статора</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F16A.5123</t>
+          <t>S17A.6113</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -510,6 +510,21 @@
       <c r="E2" t="n">
         <v>50</v>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>OP10</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Ленточнопильная</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>FMB</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>10</t>
@@ -517,7 +532,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>5,5</t>
+          <t>2,0</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -527,6 +542,21 @@
       </c>
     </row>
     <row r="3">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>OP40</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Зачистная</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Bomar Single</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>10</t>
@@ -544,138 +574,66 @@
       </c>
     </row>
     <row r="4">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>OP350</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Очистка и консервахция</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>ELMA Xхtra line AM</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>15,0</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="5">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>OP360</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Укладка в складскую тару</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Packager's WorkPlace</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>0,25</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>6,0</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>0,25</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
           <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>OP80</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>OP90</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>OP80</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>OP90</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>10</t>
         </is>
       </c>
     </row>

</xml_diff>